<commit_message>
les autres documents correspondant aux commit précédent
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/274365e861f80480/Documents/MIASHS/L3/Projet/Projet_L3/Projet-L3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/274365e861f80480/Documents/MIASHS/L3/Projet/Projet-L3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{C56647C5-1608-E741-A9A9-1DEE13D7DF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B298549E-6CB2-4233-BC81-6A1CBA73F571}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{C56647C5-1608-E741-A9A9-1DEE13D7DF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37C8A39A-C35E-4046-9618-857BFFE0D68D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{085FB95B-D901-A344-BB28-B04E529291AA}"/>
   </bookViews>
@@ -707,8 +707,8 @@
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{B176AA8C-FF81-5C4C-9C9E-236227FC730D}" name="Country"/>
-    <tableColumn id="11" xr3:uid="{B39B9EEC-93B9-4925-8CF6-726240C02458}" name="Id_Continent" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{8548E8CA-666F-6245-9937-71E70BFB2F2E}" name="Continent" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{B39B9EEC-93B9-4925-8CF6-726240C02458}" name="Id_Continent" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{8548E8CA-666F-6245-9937-71E70BFB2F2E}" name="Continent" dataDxfId="1"/>
     <tableColumn id="15" xr3:uid="{389F7008-C8BF-4565-B5F3-3B85CE9F79EE}" name="Id_Region" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{5C368F46-1F15-4B43-88C4-E5E74CE0E5B6}" name="Region"/>
     <tableColumn id="3" xr3:uid="{B2E8E2E0-997E-F742-B2A2-8D74427578A8}" name="Happiness Rank"/>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B2DD14-A70F-6F47-9A3E-8CA0A04E3006}">
   <dimension ref="A1:P783"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -18488,8 +18488,8 @@
       <c r="D349" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E349" s="1" t="e">
-        <v>#N/A</v>
+      <c r="E349" s="1">
+        <v>0</v>
       </c>
       <c r="F349" t="e">
         <v>#N/A</v>
@@ -20426,8 +20426,8 @@
       <c r="D387" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E387" s="1" t="e">
-        <v>#N/A</v>
+      <c r="E387" s="1">
+        <v>0</v>
       </c>
       <c r="F387" t="e">
         <v>#N/A</v>
@@ -26647,8 +26647,8 @@
       <c r="D509" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E509" s="1" t="e">
-        <v>#N/A</v>
+      <c r="E509" s="1">
+        <v>0</v>
       </c>
       <c r="F509" t="e">
         <v>#N/A</v>
@@ -27667,8 +27667,8 @@
       <c r="D529" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E529" s="1" t="e">
-        <v>#N/A</v>
+      <c r="E529" s="1">
+        <v>0</v>
       </c>
       <c r="F529" t="e">
         <v>#N/A</v>
@@ -34616,8 +34616,8 @@
       <c r="D666" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E666" s="1" t="e">
-        <v>#N/A</v>
+      <c r="E666" s="1">
+        <v>0</v>
       </c>
       <c r="F666" t="e">
         <v>#N/A</v>
@@ -35866,8 +35866,8 @@
       <c r="D691" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E691" s="1" t="e">
-        <v>#N/A</v>
+      <c r="E691" s="1">
+        <v>0</v>
       </c>
       <c r="F691" t="e">
         <v>#N/A</v>
@@ -36866,8 +36866,8 @@
       <c r="D711" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E711" s="1" t="e">
-        <v>#N/A</v>
+      <c r="E711" s="1">
+        <v>0</v>
       </c>
       <c r="F711" t="e">
         <v>#N/A</v>
@@ -38666,8 +38666,8 @@
       <c r="D747" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E747" s="1" t="e">
-        <v>#N/A</v>
+      <c r="E747" s="1">
+        <v>0</v>
       </c>
       <c r="F747" t="e">
         <v>#N/A</v>

</xml_diff>